<commit_message>
Wrote my first UFT script and added a wait counter
</commit_message>
<xml_diff>
--- a/uft-one-ai-ppm-strategic-portfolio-what-if/Default.xlsx
+++ b/uft-one-ai-ppm-strategic-portfolio-what-if/Default.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="01 Login" sheetId="2" r:id="rId2"/>
+    <sheet name="02 View the Advantage Portfolio" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -203,8 +204,12 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -212,12 +217,8 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -232,15 +233,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,16 +551,16 @@
     <col min="3" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="6" customFormat="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" ht="14.95" s="2" customFormat="1">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -575,7 +576,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -588,4 +589,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Strategy Tab in Portfolio Module
</commit_message>
<xml_diff>
--- a/uft-one-ai-ppm-strategic-portfolio-what-if/Default.xlsx
+++ b/uft-one-ai-ppm-strategic-portfolio-what-if/Default.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="01 Login" sheetId="2" r:id="rId2"/>
     <sheet name="02 View the Advantage Portfolio" sheetId="3" r:id="rId3"/>
+    <sheet name="03 Strategy Tab" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -182,9 +183,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -207,9 +206,7 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -217,8 +214,12 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -233,15 +234,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,11 +552,11 @@
     <col min="3" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="2" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" ht="14.95" s="3" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -563,7 +564,7 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -595,6 +596,25 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>

</xml_diff>